<commit_message>
Actualizacion de encabezados y alertas
</commit_message>
<xml_diff>
--- a/src/stock.xlsx
+++ b/src/stock.xlsx
@@ -458,16 +458,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>002</t>
+          <t>789</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Leche</t>
+          <t>Coca-Cola 500ml</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>

</xml_diff>